<commit_message>
Update to ooxml embeding from bug #45018 from Yury
git-svn-id: https://svn.apache.org/repos/asf/poi/branches/ooxml@660945 13f79535-47bb-0310-9956-ffa450edef68
</commit_message>
<xml_diff>
--- a/src/ooxml/testcases/org/apache/poi/ooxml/data/ExcelWithAttachments.xlsx
+++ b/src/ooxml/testcases/org/apache/poi/ooxml/data/ExcelWithAttachments.xlsx
@@ -919,8 +919,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1065,13 +1065,15 @@
     <hyperlink ref="E17" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
   <headerFooter alignWithMargins="0"/>
-  <drawing r:id="rId4"/>
-  <legacyDrawing r:id="rId5"/>
+  <drawing r:id="rId5"/>
+  <legacyDrawing r:id="rId6"/>
   <oleObjects>
-    <oleObject progId="MSGraph.Chart.8" shapeId="1032" r:id="rId6"/>
-    <oleObject progId="Word.Document.8" dvAspect="DVASPECT_ICON" shapeId="1033" r:id="rId7"/>
-    <oleObject progId="Word.Document.8" shapeId="1036" r:id="rId8"/>
+    <oleObject progId="MSGraph.Chart.8" shapeId="1032" r:id="rId7"/>
+    <oleObject progId="Word.Document.8" dvAspect="DVASPECT_ICON" shapeId="1033" r:id="rId8"/>
+    <oleObject progId="Word.Document.8" shapeId="1036" r:id="rId9"/>
+    <oleObject progId="PowerPoint.Show.12" shapeId="1038" r:id="rId10"/>
   </oleObjects>
 </worksheet>
 </file>

</xml_diff>